<commit_message>
Unity now switches Feeds when Matlab detects a marker in an image
</commit_message>
<xml_diff>
--- a/Docs/Unity Gantt Chart.xlsx
+++ b/Docs/Unity Gantt Chart.xlsx
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:BV25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1099,7 +1099,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="10">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="30" t="s">
@@ -1580,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G9" s="6">
         <v>0.5</v>
@@ -1660,7 +1660,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G13" s="6">
         <v>0.5</v>
@@ -1680,10 +1680,10 @@
         <v>10</v>
       </c>
       <c r="F14" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14" s="6">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1714,10 +1714,10 @@
         <v>11</v>
       </c>
       <c r="F16" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added a Kill signal to unity Added the Matlab Runtime Executable Added First Time configuration to Main.sh
</commit_message>
<xml_diff>
--- a/Docs/Unity Gantt Chart.xlsx
+++ b/Docs/Unity Gantt Chart.xlsx
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:BV25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1099,7 +1099,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="10">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="30" t="s">
@@ -1580,10 +1580,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G9" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1680,10 +1680,10 @@
         <v>10</v>
       </c>
       <c r="F14" s="5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G14" s="6">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1714,10 +1714,10 @@
         <v>11</v>
       </c>
       <c r="F16" s="5">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G16" s="6">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1730,9 +1730,15 @@
       <c r="D17" s="19">
         <v>25</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="E17" s="19">
+        <v>23</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">

</xml_diff>